<commit_message>
Ics_vendol changed to ics_shaw
</commit_message>
<xml_diff>
--- a/bin/print/TransactionReport.xlsx
+++ b/bin/print/TransactionReport.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ICS_Vendol\bin\print\ori\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
@@ -15,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Daily_Report1" localSheetId="0">Sheet1!$A$1:$N$591</definedName>
+    <definedName name="Daily_Report1" localSheetId="0">Sheet1!$A$1:$N$6</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -23,7 +18,7 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="Daily_Report" type="6" refreshedVersion="0" background="1" refreshOnLoad="1">
+  <connection id="1" name="Daily_Report" type="6" refreshedVersion="4" background="1" refreshOnLoad="1">
     <textPr prompt="0" codePage="437" sourceFile="E:\ICS_Vendol\bin\print\TransactionReport.txt" tab="0" delimiter="|">
       <textFields count="14">
         <textField/>
@@ -138,7 +133,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -172,6 +167,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -249,7 +245,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -284,7 +280,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -493,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M591"/>
+  <dimension ref="A1:O591"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="90" zoomScaleNormal="100" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:M588"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -505,17 +501,19 @@
     <col min="2" max="2" width="5.85546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="29" style="3" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" style="4" customWidth="1"/>
-    <col min="5" max="9" width="9" style="7" customWidth="1"/>
-    <col min="10" max="13" width="11.42578125" style="7" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="5" width="9" style="4" customWidth="1"/>
+    <col min="6" max="7" width="8.140625" style="7" customWidth="1"/>
+    <col min="8" max="10" width="7.85546875" style="7" customWidth="1"/>
+    <col min="11" max="14" width="10.28515625" style="7" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="14" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="14" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11"/>
       <c r="B1" s="11"/>
       <c r="C1" s="12"/>
       <c r="D1" s="13"/>
-      <c r="E1" s="10"/>
+      <c r="E1" s="13"/>
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
@@ -524,8 +522,10 @@
       <c r="K1" s="10"/>
       <c r="L1" s="10"/>
       <c r="M1" s="10"/>
-    </row>
-    <row r="2" spans="1:13" s="9" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N1" s="10"/>
+      <c r="O1" s="15"/>
+    </row>
+    <row r="2" spans="1:15" s="9" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -539,44 +539,52 @@
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
-    </row>
-    <row r="4" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N2" s="6"/>
+      <c r="O2" s="15"/>
+    </row>
+    <row r="3" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O3" s="15"/>
+    </row>
+    <row r="4" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="5"/>
-    </row>
-    <row r="5" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O4" s="15"/>
+    </row>
+    <row r="5" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="5"/>
-    </row>
-    <row r="6" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O5" s="15"/>
+    </row>
+    <row r="6" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="5"/>
-    </row>
-    <row r="7" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O6" s="15"/>
+    </row>
+    <row r="7" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C15" s="5"/>
     </row>
-    <row r="16" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C16" s="5"/>
     </row>
     <row r="17" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2259,78 +2267,58 @@
     <row r="576" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C576" s="5"/>
     </row>
-    <row r="577" spans="3:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="577" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C577" s="5"/>
     </row>
-    <row r="578" spans="3:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="578" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C578" s="5"/>
     </row>
-    <row r="579" spans="3:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="579" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C579" s="5"/>
     </row>
-    <row r="580" spans="3:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="580" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C580" s="5"/>
     </row>
-    <row r="581" spans="3:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="581" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C581" s="5"/>
     </row>
-    <row r="582" spans="3:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="582" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C582" s="5"/>
     </row>
-    <row r="583" spans="3:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="583" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C583" s="5"/>
     </row>
-    <row r="584" spans="3:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="584" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C584" s="5"/>
     </row>
-    <row r="585" spans="3:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="585" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C585" s="5"/>
     </row>
-    <row r="586" spans="3:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="586" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C586" s="5"/>
     </row>
-    <row r="587" spans="3:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="587" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C587" s="5"/>
     </row>
-    <row r="588" spans="3:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="588" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C588" s="5"/>
     </row>
-    <row r="589" spans="3:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="589" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C589" s="5"/>
     </row>
-    <row r="590" spans="3:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="590" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C590" s="5"/>
-      <c r="D590" s="4"/>
-      <c r="E590" s="7"/>
-      <c r="F590" s="7"/>
-      <c r="G590" s="7"/>
-      <c r="H590" s="7"/>
-      <c r="I590" s="7"/>
-      <c r="J590" s="7"/>
-      <c r="K590" s="7"/>
-      <c r="L590" s="7"/>
-      <c r="M590" s="7"/>
-    </row>
-    <row r="591" spans="3:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="591" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C591" s="5"/>
-      <c r="D591" s="4"/>
-      <c r="E591" s="7"/>
-      <c r="F591" s="7"/>
-      <c r="G591" s="7"/>
-      <c r="H591" s="7"/>
-      <c r="I591" s="7"/>
-      <c r="J591" s="7"/>
-      <c r="K591" s="7"/>
-      <c r="L591" s="7"/>
-      <c r="M591" s="7"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E1:L1048576">
+  <conditionalFormatting sqref="F1:M1048576">
     <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M1:M1048576">
+  <conditionalFormatting sqref="N1:N1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>